<commit_message>
Author: hungbk99 - connection
</commit_message>
<xml_diff>
--- a/AMBA_BUS/AHB_GEN_202/Input/AHB_config.xlsx
+++ b/AMBA_BUS/AHB_GEN_202/Input/AHB_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Decoder_config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>AHB_Gen Decoder Setting</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>master_data</t>
-  </si>
-  <si>
-    <t>slave_isnt</t>
   </si>
 </sst>
 </file>
@@ -861,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +974,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1061,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>